<commit_message>
cosas chicas arregladas en editar SKUs (tanto manual como a traves de archivo) y algunas cosas en consola
</commit_message>
<xml_diff>
--- a/Hojas de parametros estandar/Purchases.xlsx
+++ b/Hojas de parametros estandar/Purchases.xlsx
@@ -16,9 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -29,6 +26,9 @@
   </si>
   <si>
     <t>Arrival Day</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
   <dimension ref="B2:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -476,19 +476,19 @@
   <sheetData>
     <row r="2" spans="2:6">
       <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:6">

</xml_diff>